<commit_message>
I prefer lower-case names
</commit_message>
<xml_diff>
--- a/spank.xlsx
+++ b/spank.xlsx
@@ -29,30 +29,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="115">
   <si>
-    <t>Study</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Outcome</t>
-  </si>
-  <si>
-    <t>Between</t>
-  </si>
-  <si>
-    <t>Within</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
-    <t>LL</t>
-  </si>
-  <si>
-    <t>UL</t>
-  </si>
-  <si>
     <t>Bean and Roberts (1981)</t>
   </si>
   <si>
@@ -372,6 +351,27 @@
   </si>
   <si>
     <t>Graziano et al. (1992) India sample</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>between</t>
+  </si>
+  <si>
+    <t>within</t>
+  </si>
+  <si>
+    <t>ll</t>
+  </si>
+  <si>
+    <t>ul</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
   <dimension ref="A1:H112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,39 +725,39 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>108</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>110</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>7</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5">
         <v>1981</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
@@ -777,13 +777,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5">
         <v>1983</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -803,13 +803,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B4" s="5">
         <v>1971</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D4" s="5">
         <v>0</v>
@@ -829,13 +829,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B5" s="5">
         <v>1988</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
@@ -855,13 +855,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5">
         <v>1990</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
@@ -881,13 +881,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>1961</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D7" s="5">
         <v>0</v>
@@ -907,13 +907,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B8" s="5">
         <v>1962</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
@@ -933,13 +933,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B9" s="5">
         <v>1990</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D9" s="5">
         <v>0</v>
@@ -959,13 +959,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B10" s="5">
         <v>2002</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D10" s="5">
         <v>0</v>
@@ -985,13 +985,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B11" s="5">
         <v>2005</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D11" s="5">
         <v>0</v>
@@ -1011,13 +1011,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B12" s="5">
         <v>1986</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
@@ -1037,13 +1037,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B13" s="5">
         <v>2012</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D13" s="5">
         <v>0</v>
@@ -1063,13 +1063,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B14" s="5">
         <v>1979</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
@@ -1089,13 +1089,13 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B15" s="5">
         <v>2009</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D15" s="5">
         <v>0</v>
@@ -1115,13 +1115,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B16" s="5">
         <v>2010</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D16" s="5">
         <v>0</v>
@@ -1141,13 +1141,13 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5">
         <v>1997</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D17" s="5">
         <v>0</v>
@@ -1167,13 +1167,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B18" s="5">
         <v>1990</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D18" s="5">
         <v>0</v>
@@ -1193,13 +1193,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B19" s="5">
         <v>2004</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D19" s="5">
         <v>1</v>
@@ -1219,13 +1219,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B20" s="5">
         <v>1961</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D20" s="5">
         <v>0</v>
@@ -1245,13 +1245,13 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B21" s="5">
         <v>2013</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D21" s="5">
         <v>0</v>
@@ -1271,13 +1271,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B22" s="5">
         <v>2011</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D22" s="5">
         <v>0</v>
@@ -1297,13 +1297,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B23" s="5">
         <v>1999</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
@@ -1323,13 +1323,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B24" s="5">
         <v>1997</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D24" s="5">
         <v>0</v>
@@ -1349,13 +1349,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B25" s="5">
         <v>2010</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D25" s="5">
         <v>0</v>
@@ -1375,13 +1375,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B26" s="5">
         <v>1995</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D26" s="5">
         <v>1</v>
@@ -1401,13 +1401,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B27" s="5">
         <v>2004</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D27" s="5">
         <v>0</v>
@@ -1427,13 +1427,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B28" s="5">
         <v>2005</v>
       </c>
       <c r="C28" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D28" s="5">
         <v>0</v>
@@ -1453,13 +1453,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B29" s="5">
         <v>2004</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
@@ -1479,13 +1479,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B30" s="5">
         <v>1997</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D30" s="5">
         <v>0</v>
@@ -1505,13 +1505,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B31" s="5">
         <v>2009</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D31" s="5">
         <v>1</v>
@@ -1531,13 +1531,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B32" s="5">
         <v>2013</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D32" s="5">
         <v>0</v>
@@ -1557,13 +1557,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B33" s="5">
         <v>2013</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D33" s="5">
         <v>0</v>
@@ -1583,13 +1583,13 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B34" s="5">
         <v>2009</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D34" s="5">
         <v>0</v>
@@ -1609,13 +1609,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B35" s="5">
         <v>2012</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D35" s="5">
         <v>0</v>
@@ -1635,13 +1635,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B36" s="5">
         <v>2011</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D36" s="5">
         <v>0</v>
@@ -1661,13 +1661,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B37" s="5">
         <v>2012</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D37" s="5">
         <v>0</v>
@@ -1687,13 +1687,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B38" s="5">
         <v>2012</v>
       </c>
       <c r="C38" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D38" s="5">
         <v>0</v>
@@ -1713,13 +1713,13 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B39" s="5">
         <v>2007</v>
       </c>
       <c r="C39" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D39" s="5">
         <v>0</v>
@@ -1739,13 +1739,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B40" s="5">
         <v>1993</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D40" s="5">
         <v>0</v>
@@ -1765,13 +1765,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B41" s="5">
         <v>2007</v>
       </c>
       <c r="C41" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D41" s="5">
         <v>0</v>
@@ -1791,13 +1791,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B42" s="5">
         <v>2002</v>
       </c>
       <c r="C42" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D42" s="5">
         <v>0</v>
@@ -1817,13 +1817,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B43" s="5">
         <v>2012</v>
       </c>
       <c r="C43" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D43" s="5">
         <v>0</v>
@@ -1843,13 +1843,13 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B44" s="5">
         <v>2013</v>
       </c>
       <c r="C44" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D44" s="5">
         <v>0</v>
@@ -1869,13 +1869,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B45" s="5">
         <v>2009</v>
       </c>
       <c r="C45" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D45" s="5">
         <v>1</v>
@@ -1895,13 +1895,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B46" s="5">
         <v>2009</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D46" s="5">
         <v>0</v>
@@ -1921,13 +1921,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B47" s="5">
         <v>2010</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D47" s="5">
         <v>0</v>
@@ -1947,13 +1947,13 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B48" s="5">
         <v>2011</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D48" s="5">
         <v>0</v>
@@ -1973,13 +1973,13 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B49" s="5">
         <v>2010</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D49" s="5">
         <v>1</v>
@@ -1999,13 +1999,13 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B50" s="5">
         <v>2012</v>
       </c>
       <c r="C50" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D50" s="5">
         <v>0</v>
@@ -2025,13 +2025,13 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B51" s="5">
         <v>2007</v>
       </c>
       <c r="C51" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D51" s="5">
         <v>0</v>
@@ -2051,13 +2051,13 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B52" s="5">
         <v>1993</v>
       </c>
       <c r="C52" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D52" s="5">
         <v>0</v>
@@ -2077,13 +2077,13 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B53" s="5">
         <v>2002</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D53" s="5">
         <v>0</v>
@@ -2103,13 +2103,13 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B54" s="5">
         <v>2003</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D54" s="5">
         <v>0</v>
@@ -2129,13 +2129,13 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B55" s="5">
         <v>2008</v>
       </c>
       <c r="C55" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D55" s="5">
         <v>0</v>
@@ -2155,13 +2155,13 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B56" s="5">
         <v>1990</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D56" s="5">
         <v>0</v>
@@ -2181,13 +2181,13 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B57" s="5">
         <v>2004</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D57" s="5">
         <v>0</v>
@@ -2207,13 +2207,13 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B58" s="5">
         <v>2003</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D58" s="5">
         <v>1</v>
@@ -2233,13 +2233,13 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B59" s="5">
         <v>2001</v>
       </c>
       <c r="C59" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D59" s="5">
         <v>1</v>
@@ -2259,13 +2259,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B60" s="5">
         <v>2009</v>
       </c>
       <c r="C60" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D60" s="5">
         <v>0</v>
@@ -2285,13 +2285,13 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B61" s="5">
         <v>2007</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D61" s="5">
         <v>0</v>
@@ -2311,13 +2311,13 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B62" s="5">
         <v>1961</v>
       </c>
       <c r="C62" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D62" s="5">
         <v>0</v>
@@ -2337,13 +2337,13 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B63" s="5">
         <v>2010</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D63" s="5">
         <v>1</v>
@@ -2363,13 +2363,13 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B64" s="5">
         <v>2003</v>
       </c>
       <c r="C64" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D64" s="5">
         <v>1</v>
@@ -2389,13 +2389,13 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B65" s="5">
         <v>2005</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D65" s="5">
         <v>1</v>
@@ -2415,13 +2415,13 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B66" s="5">
         <v>2002</v>
       </c>
       <c r="C66" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D66" s="5">
         <v>0</v>
@@ -2441,13 +2441,13 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B67" s="5">
         <v>1991</v>
       </c>
       <c r="C67" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D67" s="5">
         <v>0</v>
@@ -2467,13 +2467,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B68" s="5">
         <v>1990</v>
       </c>
       <c r="C68" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D68" s="5">
         <v>0</v>
@@ -2493,13 +2493,13 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B69" s="5">
         <v>1989</v>
       </c>
       <c r="C69" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D69" s="5">
         <v>0</v>
@@ -2519,13 +2519,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B70" s="5">
         <v>2001</v>
       </c>
       <c r="C70" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D70" s="5">
         <v>0</v>
@@ -2545,13 +2545,13 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B71" s="5">
         <v>2009</v>
       </c>
       <c r="C71" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D71" s="5">
         <v>0</v>
@@ -2571,13 +2571,13 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B72" s="5">
         <v>2004</v>
       </c>
       <c r="C72" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D72" s="5">
         <v>0</v>
@@ -2597,13 +2597,13 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B73" s="5">
         <v>2009</v>
       </c>
       <c r="C73" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D73" s="5">
         <v>0</v>
@@ -2623,13 +2623,13 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B74" s="5">
         <v>2012</v>
       </c>
       <c r="C74" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D74" s="5">
         <v>0</v>
@@ -2649,13 +2649,13 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B75" s="5">
         <v>2005</v>
       </c>
       <c r="C75" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D75" s="5">
         <v>0</v>
@@ -2675,13 +2675,13 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B76" s="5">
         <v>1982</v>
       </c>
       <c r="C76" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D76" s="5">
         <v>0</v>
@@ -2701,13 +2701,13 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B77" s="5">
         <v>1986</v>
       </c>
       <c r="C77" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D77" s="5">
         <v>1</v>
@@ -2727,13 +2727,13 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B78" s="5">
         <v>2009</v>
       </c>
       <c r="C78" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D78" s="5">
         <v>0</v>
@@ -2753,13 +2753,13 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B79" s="5">
         <v>1991</v>
       </c>
       <c r="C79" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D79" s="5">
         <v>0</v>
@@ -2779,13 +2779,13 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B80" s="5">
         <v>2003</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D80" s="5">
         <v>1</v>
@@ -2805,13 +2805,13 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B81" s="5">
         <v>2013</v>
       </c>
       <c r="C81" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D81" s="5">
         <v>1</v>
@@ -2831,13 +2831,13 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B82" s="5">
         <v>2011</v>
       </c>
       <c r="C82" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D82" s="5">
         <v>0</v>
@@ -2857,13 +2857,13 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B83" s="5">
         <v>2009</v>
       </c>
       <c r="C83" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D83" s="5">
         <v>0</v>
@@ -2883,13 +2883,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B84" s="5">
         <v>2009</v>
       </c>
       <c r="C84" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D84" s="5">
         <v>0</v>
@@ -2909,13 +2909,13 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B85" s="5">
         <v>2003</v>
       </c>
       <c r="C85" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D85" s="5">
         <v>0</v>
@@ -2935,13 +2935,13 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B86" s="5">
         <v>2005</v>
       </c>
       <c r="C86" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D86" s="5">
         <v>0</v>
@@ -2961,13 +2961,13 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B87" s="5">
         <v>2002</v>
       </c>
       <c r="C87" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D87" s="5">
         <v>1</v>
@@ -2987,13 +2987,13 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B88" s="5">
         <v>2007</v>
       </c>
       <c r="C88" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D88" s="5">
         <v>0</v>
@@ -3013,13 +3013,13 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B89" s="5">
         <v>1994</v>
       </c>
       <c r="C89" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D89" s="5">
         <v>1</v>
@@ -3039,13 +3039,13 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B90" s="5">
         <v>1981</v>
       </c>
       <c r="C90" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D90" s="5">
         <v>0</v>
@@ -3065,13 +3065,13 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B91" s="5">
         <v>1986</v>
       </c>
       <c r="C91" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D91" s="5">
         <v>1</v>
@@ -3091,13 +3091,13 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B92" s="5">
         <v>2008</v>
       </c>
       <c r="C92" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D92" s="5">
         <v>1</v>
@@ -3117,13 +3117,13 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B93" s="5">
         <v>2008</v>
       </c>
       <c r="C93" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D93" s="5">
         <v>1</v>
@@ -3143,13 +3143,13 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B94" s="5">
         <v>2006</v>
       </c>
       <c r="C94" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D94" s="5">
         <v>1</v>
@@ -3169,13 +3169,13 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B95" s="5">
         <v>1991</v>
       </c>
       <c r="C95" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D95" s="5">
         <v>1</v>
@@ -3195,13 +3195,13 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B96" s="5">
         <v>2008</v>
       </c>
       <c r="C96" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D96" s="5">
         <v>1</v>
@@ -3221,13 +3221,13 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B97" s="5">
         <v>1992</v>
       </c>
       <c r="C97" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D97" s="5">
         <v>0</v>
@@ -3247,13 +3247,13 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B98" s="5">
         <v>2006</v>
       </c>
       <c r="C98" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D98" s="5">
         <v>1</v>
@@ -3273,13 +3273,13 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B99" s="5">
         <v>2001</v>
       </c>
       <c r="C99" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D99" s="5">
         <v>0</v>
@@ -3299,13 +3299,13 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B100" s="5">
         <v>2009</v>
       </c>
       <c r="C100" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D100" s="5">
         <v>0</v>
@@ -3325,13 +3325,13 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B101" s="5">
         <v>1996</v>
       </c>
       <c r="C101" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D101" s="5">
         <v>1</v>
@@ -3351,13 +3351,13 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B102" s="5">
         <v>2011</v>
       </c>
       <c r="C102" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D102" s="5">
         <v>0</v>
@@ -3377,13 +3377,13 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B103" s="5">
         <v>2013</v>
       </c>
       <c r="C103" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D103" s="5">
         <v>1</v>
@@ -3403,13 +3403,13 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B104" s="5">
         <v>1974</v>
       </c>
       <c r="C104" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D104" s="5">
         <v>1</v>
@@ -3429,13 +3429,13 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B105" s="5">
         <v>2008</v>
       </c>
       <c r="C105" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D105" s="5">
         <v>1</v>
@@ -3455,13 +3455,13 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B106" s="5">
         <v>2006</v>
       </c>
       <c r="C106" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D106" s="5">
         <v>1</v>
@@ -3481,13 +3481,13 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B107" s="5">
         <v>1975</v>
       </c>
       <c r="C107" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D107" s="5">
         <v>1</v>
@@ -3507,13 +3507,13 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B108" s="5">
         <v>2006</v>
       </c>
       <c r="C108" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D108" s="5">
         <v>1</v>
@@ -3533,13 +3533,13 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B109" s="5">
         <v>1993</v>
       </c>
       <c r="C109" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D109" s="5">
         <v>1</v>
@@ -3559,13 +3559,13 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B110" s="5">
         <v>1992</v>
       </c>
       <c r="C110" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D110" s="5">
         <v>0</v>
@@ -3585,13 +3585,13 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B111" s="5">
         <v>1992</v>
       </c>
       <c r="C111" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D111" s="5">
         <v>0</v>
@@ -3611,13 +3611,13 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B112" s="5">
         <v>1994</v>
       </c>
       <c r="C112" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D112" s="5">
         <v>1</v>

</xml_diff>